<commit_message>
Sua sdt a.Trung va Thanh Thanh, them cac file cua bdh cu
</commit_message>
<xml_diff>
--- a/2019/danh sach mien 2019/DANH SÁCH MIỀN NĂM HỌC 2019-2020.xlsx
+++ b/2019/danh sach mien 2019/DANH SÁCH MIỀN NĂM HỌC 2019-2020.xlsx
@@ -339,9 +339,6 @@
     <t>0329 775 627</t>
   </si>
   <si>
-    <t>0582 247 685</t>
-  </si>
-  <si>
     <t>0397 145 599</t>
   </si>
   <si>
@@ -352,9 +349,6 @@
   </si>
   <si>
     <t>0367 019 655</t>
-  </si>
-  <si>
-    <t>0338 040 075</t>
   </si>
   <si>
     <t>0783 808 147</t>
@@ -548,6 +542,12 @@
   <si>
     <t>Đổ Trọng</t>
   </si>
+  <si>
+    <t>033 932 1365</t>
+  </si>
+  <si>
+    <t>034 790 1808</t>
+  </si>
 </sst>
 </file>
 
@@ -557,7 +557,7 @@
     <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="#,##0.000;[Red]#,##0.000"/>
     <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="169" formatCode="#,##0.000"/>
+    <numFmt numFmtId="167" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -657,22 +657,21 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color theme="0"/>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="163"/>
     </font>
     <font>
       <b/>
-      <sz val="9"/>
-      <color rgb="FFFF0000"/>
+      <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="163"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -682,6 +681,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -826,7 +831,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -853,7 +858,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -995,29 +1000,11 @@
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="14" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1031,9 +1018,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1087,6 +1071,33 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1097,7 +1108,7 @@
   <dxfs count="13">
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1106,25 +1117,27 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="9"/>
+        <sz val="10"/>
         <color auto="1"/>
         <name val="Times New Roman"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1167,7 +1180,7 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1176,27 +1189,26 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="0"/>
+        <sz val="9"/>
+        <color auto="1"/>
         <name val="Times New Roman"/>
         <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <numFmt numFmtId="165" formatCode="#,##0.000;[Red]#,##0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1215,7 +1227,6 @@
         <name val="Times New Roman"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="#,##0.000;[Red]#,##0.000"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1478,7 +1489,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="D3:L36" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" headerRowBorderDxfId="1" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="D3:L36" totalsRowShown="0" headerRowDxfId="0" dataDxfId="3" headerRowBorderDxfId="1" tableBorderDxfId="2">
   <autoFilter ref="D3:L36"/>
   <sortState ref="D4:L36">
     <sortCondition ref="K3:K36"/>
@@ -1491,8 +1502,8 @@
     <tableColumn id="6" name="Ngành Học / Trường Học" dataDxfId="8"/>
     <tableColumn id="7" name="Điện Thoại" dataDxfId="7"/>
     <tableColumn id="8" name="Niên khóa" dataDxfId="6"/>
-    <tableColumn id="10" name="Đội" dataDxfId="0"/>
-    <tableColumn id="9" name="Ghi Chú" dataDxfId="5"/>
+    <tableColumn id="10" name="Đội" dataDxfId="5"/>
+    <tableColumn id="9" name="Ghi Chú" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1788,7 +1799,7 @@
   <dimension ref="C1:N72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1808,68 +1819,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:14" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="78" t="s">
-        <v>131</v>
-      </c>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
+      <c r="D1" s="106" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="106"/>
+      <c r="F1" s="106"/>
+      <c r="G1" s="106"/>
+      <c r="H1" s="106"/>
+      <c r="I1" s="106"/>
+      <c r="J1" s="106"/>
+      <c r="K1" s="106"/>
+      <c r="L1" s="106"/>
       <c r="M1" s="74"/>
       <c r="N1" s="74"/>
     </row>
     <row r="2" spans="3:14" s="2" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="M2" s="110"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="106"/>
+      <c r="J2" s="106"/>
+      <c r="K2" s="106"/>
+      <c r="L2" s="106"/>
+      <c r="M2" s="103"/>
       <c r="N2" s="73"/>
     </row>
     <row r="3" spans="3:14" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="111" t="s">
+      <c r="C3" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="81" t="s">
-        <v>141</v>
-      </c>
-      <c r="E3" s="82" t="s">
+      <c r="D3" s="109" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" s="111" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="112" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="112" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="112" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="113" t="s">
+        <v>121</v>
+      </c>
+      <c r="K3" s="114" t="s">
+        <v>131</v>
+      </c>
+      <c r="L3" s="109" t="s">
         <v>132</v>
       </c>
-      <c r="F3" s="83" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="84" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="84" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="84" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="85" t="s">
-        <v>123</v>
-      </c>
-      <c r="K3" s="92" t="s">
-        <v>133</v>
-      </c>
-      <c r="L3" s="81" t="s">
-        <v>134</v>
-      </c>
       <c r="M3" s="75"/>
     </row>
     <row r="4" spans="3:14" s="2" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="112">
+      <c r="C4" s="105">
         <v>1</v>
       </c>
       <c r="D4" s="28" t="s">
@@ -1888,21 +1899,21 @@
         <v>18</v>
       </c>
       <c r="I4" s="31" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J4" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="93">
+      <c r="K4" s="86">
         <v>1</v>
       </c>
-      <c r="L4" s="79" t="s">
-        <v>144</v>
+      <c r="L4" s="78" t="s">
+        <v>142</v>
       </c>
       <c r="M4" s="25"/>
     </row>
     <row r="5" spans="3:14" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="112">
+      <c r="C5" s="105">
         <v>2</v>
       </c>
       <c r="D5" s="38" t="s">
@@ -1926,16 +1937,16 @@
       <c r="J5" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="95">
+      <c r="K5" s="88">
         <v>1</v>
       </c>
-      <c r="L5" s="79" t="s">
-        <v>145</v>
+      <c r="L5" s="78" t="s">
+        <v>143</v>
       </c>
       <c r="M5" s="25"/>
     </row>
     <row r="6" spans="3:14" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="112">
+      <c r="C6" s="105">
         <v>3</v>
       </c>
       <c r="D6" s="38" t="s">
@@ -1959,14 +1970,14 @@
       <c r="J6" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="K6" s="95">
+      <c r="K6" s="88">
         <v>1</v>
       </c>
-      <c r="L6" s="79"/>
+      <c r="L6" s="78"/>
       <c r="M6" s="25"/>
     </row>
     <row r="7" spans="3:14" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="112">
+      <c r="C7" s="105">
         <v>4</v>
       </c>
       <c r="D7" s="53" t="s">
@@ -1982,22 +1993,22 @@
         <v>15</v>
       </c>
       <c r="H7" s="57" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I7" s="56" t="s">
         <v>101</v>
       </c>
       <c r="J7" s="46" t="s">
-        <v>121</v>
-      </c>
-      <c r="K7" s="96">
+        <v>119</v>
+      </c>
+      <c r="K7" s="89">
         <v>1</v>
       </c>
-      <c r="L7" s="79"/>
+      <c r="L7" s="78"/>
       <c r="M7" s="25"/>
     </row>
     <row r="8" spans="3:14" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="112">
+      <c r="C8" s="105">
         <v>5</v>
       </c>
       <c r="D8" s="53" t="s">
@@ -2021,14 +2032,14 @@
       <c r="J8" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="K8" s="98">
+      <c r="K8" s="91">
         <v>1</v>
       </c>
-      <c r="L8" s="79"/>
+      <c r="L8" s="78"/>
       <c r="M8" s="25"/>
     </row>
     <row r="9" spans="3:14" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="112">
+      <c r="C9" s="105">
         <v>6</v>
       </c>
       <c r="D9" s="17" t="s">
@@ -2052,45 +2063,45 @@
       <c r="J9" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="K9" s="101">
+      <c r="K9" s="94">
         <v>1</v>
       </c>
-      <c r="L9" s="79"/>
+      <c r="L9" s="78"/>
       <c r="M9" s="25"/>
     </row>
     <row r="10" spans="3:14" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="112">
+      <c r="C10" s="105">
         <v>7</v>
       </c>
-      <c r="D10" s="104" t="s">
+      <c r="D10" s="97" t="s">
         <v>72</v>
       </c>
-      <c r="E10" s="105" t="s">
+      <c r="E10" s="98" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="106">
+      <c r="F10" s="99">
         <v>36102</v>
       </c>
-      <c r="G10" s="107" t="s">
+      <c r="G10" s="100" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="108" t="s">
+      <c r="H10" s="101" t="s">
         <v>20</v>
       </c>
       <c r="I10" s="107" t="s">
-        <v>112</v>
-      </c>
-      <c r="J10" s="107" t="s">
+        <v>149</v>
+      </c>
+      <c r="J10" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="K10" s="109">
+      <c r="K10" s="102">
         <v>1</v>
       </c>
-      <c r="L10" s="79"/>
+      <c r="L10" s="78"/>
       <c r="M10" s="25"/>
     </row>
     <row r="11" spans="3:14" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="112">
+      <c r="C11" s="105">
         <v>8</v>
       </c>
       <c r="D11" s="28" t="s">
@@ -2114,14 +2125,14 @@
       <c r="J11" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="K11" s="93">
+      <c r="K11" s="86">
         <v>1</v>
       </c>
-      <c r="L11" s="79"/>
+      <c r="L11" s="78"/>
       <c r="M11" s="25"/>
     </row>
     <row r="12" spans="3:14" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="112">
+      <c r="C12" s="105">
         <v>9</v>
       </c>
       <c r="D12" s="28" t="s">
@@ -2140,19 +2151,19 @@
         <v>32</v>
       </c>
       <c r="I12" s="31" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J12" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="K12" s="93">
+      <c r="K12" s="86">
         <v>1</v>
       </c>
-      <c r="L12" s="79"/>
+      <c r="L12" s="78"/>
       <c r="M12" s="25"/>
     </row>
     <row r="13" spans="3:14" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="112">
+      <c r="C13" s="105">
         <v>10</v>
       </c>
       <c r="D13" s="28" t="s">
@@ -2176,16 +2187,16 @@
       <c r="J13" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="K13" s="93">
+      <c r="K13" s="86">
         <v>2</v>
       </c>
-      <c r="L13" s="79" t="s">
-        <v>146</v>
+      <c r="L13" s="78" t="s">
+        <v>144</v>
       </c>
       <c r="M13" s="25"/>
     </row>
     <row r="14" spans="3:14" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="112">
+      <c r="C14" s="105">
         <v>11</v>
       </c>
       <c r="D14" s="48" t="s">
@@ -2209,16 +2220,16 @@
       <c r="J14" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="K14" s="97">
+      <c r="K14" s="90">
         <v>2</v>
       </c>
-      <c r="L14" s="79" t="s">
-        <v>147</v>
+      <c r="L14" s="78" t="s">
+        <v>145</v>
       </c>
       <c r="M14" s="25"/>
     </row>
     <row r="15" spans="3:14" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="112">
+      <c r="C15" s="105">
         <v>12</v>
       </c>
       <c r="D15" s="38" t="s">
@@ -2242,14 +2253,14 @@
       <c r="J15" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="K15" s="95">
+      <c r="K15" s="88">
         <v>2</v>
       </c>
-      <c r="L15" s="79"/>
+      <c r="L15" s="78"/>
       <c r="M15" s="25"/>
     </row>
     <row r="16" spans="3:14" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="112">
+      <c r="C16" s="105">
         <v>13</v>
       </c>
       <c r="D16" s="58" t="s">
@@ -2273,45 +2284,45 @@
       <c r="J16" s="61" t="s">
         <v>77</v>
       </c>
-      <c r="K16" s="99">
+      <c r="K16" s="92">
         <v>2</v>
       </c>
-      <c r="L16" s="79"/>
+      <c r="L16" s="78"/>
       <c r="M16" s="25"/>
     </row>
     <row r="17" spans="3:13" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="112">
+      <c r="C17" s="105">
         <v>14</v>
       </c>
-      <c r="D17" s="86" t="s">
+      <c r="D17" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="87" t="s">
+      <c r="E17" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="F17" s="89">
+      <c r="F17" s="83">
         <v>36009</v>
       </c>
-      <c r="G17" s="90" t="s">
+      <c r="G17" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="91" t="s">
+      <c r="H17" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="I17" s="90" t="s">
-        <v>109</v>
-      </c>
-      <c r="J17" s="90" t="s">
+      <c r="I17" s="84" t="s">
+        <v>108</v>
+      </c>
+      <c r="J17" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="K17" s="103">
+      <c r="K17" s="96">
         <v>2</v>
       </c>
-      <c r="L17" s="79"/>
+      <c r="L17" s="78"/>
       <c r="M17" s="25"/>
     </row>
     <row r="18" spans="3:13" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="112">
+      <c r="C18" s="105">
         <v>15</v>
       </c>
       <c r="D18" s="33" t="s">
@@ -2330,23 +2341,23 @@
         <v>18</v>
       </c>
       <c r="I18" s="36" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J18" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="K18" s="94">
+      <c r="K18" s="87">
         <v>2</v>
       </c>
-      <c r="L18" s="79"/>
+      <c r="L18" s="78"/>
       <c r="M18" s="25"/>
     </row>
     <row r="19" spans="3:13" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="112">
+      <c r="C19" s="105">
         <v>16</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E19" s="34" t="s">
         <v>40</v>
@@ -2361,19 +2372,19 @@
         <v>22</v>
       </c>
       <c r="I19" s="36" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J19" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="K19" s="94">
+      <c r="K19" s="87">
         <v>2</v>
       </c>
-      <c r="L19" s="79"/>
+      <c r="L19" s="78"/>
       <c r="M19" s="25"/>
     </row>
     <row r="20" spans="3:13" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="112">
+      <c r="C20" s="105">
         <v>17</v>
       </c>
       <c r="D20" s="68" t="s">
@@ -2392,19 +2403,19 @@
         <v>18</v>
       </c>
       <c r="I20" s="31" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J20" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="K20" s="102">
+      <c r="K20" s="95">
         <v>2</v>
       </c>
-      <c r="L20" s="79"/>
+      <c r="L20" s="78"/>
       <c r="M20" s="76"/>
     </row>
     <row r="21" spans="3:13" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="112">
+      <c r="C21" s="105">
         <v>18</v>
       </c>
       <c r="D21" s="68" t="s">
@@ -2423,19 +2434,19 @@
         <v>57</v>
       </c>
       <c r="I21" s="31" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J21" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="K21" s="102">
+      <c r="K21" s="95">
         <v>2</v>
       </c>
-      <c r="L21" s="79"/>
+      <c r="L21" s="78"/>
       <c r="M21" s="25"/>
     </row>
     <row r="22" spans="3:13" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="112">
+      <c r="C22" s="105">
         <v>19</v>
       </c>
       <c r="D22" s="28" t="s">
@@ -2451,57 +2462,57 @@
         <v>51</v>
       </c>
       <c r="H22" s="32" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I22" s="31" t="s">
         <v>76</v>
       </c>
       <c r="J22" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="K22" s="93">
+        <v>126</v>
+      </c>
+      <c r="K22" s="86">
         <v>3</v>
       </c>
-      <c r="L22" s="79" t="s">
-        <v>148</v>
+      <c r="L22" s="78" t="s">
+        <v>146</v>
       </c>
       <c r="M22" s="26"/>
     </row>
     <row r="23" spans="3:13" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="112">
+      <c r="C23" s="105">
         <v>20</v>
       </c>
       <c r="D23" s="38" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E23" s="39" t="s">
-        <v>125</v>
-      </c>
-      <c r="F23" s="88">
+        <v>123</v>
+      </c>
+      <c r="F23" s="82">
         <v>36614</v>
       </c>
       <c r="G23" s="41" t="s">
         <v>15</v>
       </c>
       <c r="H23" s="42" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I23" s="41" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J23" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="K23" s="95">
+      <c r="K23" s="88">
         <v>3</v>
       </c>
-      <c r="L23" s="79" t="s">
-        <v>149</v>
+      <c r="L23" s="78" t="s">
+        <v>147</v>
       </c>
       <c r="M23" s="25"/>
     </row>
     <row r="24" spans="3:13" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="112">
+      <c r="C24" s="105">
         <v>21</v>
       </c>
       <c r="D24" s="33" t="s">
@@ -2525,16 +2536,16 @@
       <c r="J24" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="K24" s="94">
+      <c r="K24" s="87">
         <v>3</v>
       </c>
-      <c r="L24" s="79" t="s">
-        <v>143</v>
+      <c r="L24" s="78" t="s">
+        <v>141</v>
       </c>
       <c r="M24" s="26"/>
     </row>
     <row r="25" spans="3:13" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="112">
+      <c r="C25" s="105">
         <v>22</v>
       </c>
       <c r="D25" s="33" t="s">
@@ -2558,14 +2569,14 @@
       <c r="J25" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="K25" s="94">
+      <c r="K25" s="87">
         <v>3</v>
       </c>
-      <c r="L25" s="79"/>
+      <c r="L25" s="78"/>
       <c r="M25" s="26"/>
     </row>
     <row r="26" spans="3:13" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="112">
+      <c r="C26" s="105">
         <v>23</v>
       </c>
       <c r="D26" s="38" t="s">
@@ -2589,14 +2600,14 @@
       <c r="J26" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="K26" s="95">
+      <c r="K26" s="88">
         <v>3</v>
       </c>
-      <c r="L26" s="79"/>
+      <c r="L26" s="78"/>
       <c r="M26" s="26"/>
     </row>
     <row r="27" spans="3:13" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="112">
+      <c r="C27" s="105">
         <v>24</v>
       </c>
       <c r="D27" s="33" t="s">
@@ -2614,20 +2625,20 @@
       <c r="H27" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="I27" s="36" t="s">
-        <v>107</v>
+      <c r="I27" s="108" t="s">
+        <v>150</v>
       </c>
       <c r="J27" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="K27" s="94">
+      <c r="K27" s="87">
         <v>3</v>
       </c>
-      <c r="L27" s="79"/>
+      <c r="L27" s="78"/>
       <c r="M27" s="26"/>
     </row>
     <row r="28" spans="3:13" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="112">
+      <c r="C28" s="105">
         <v>25</v>
       </c>
       <c r="D28" s="63" t="s">
@@ -2646,19 +2657,19 @@
         <v>32</v>
       </c>
       <c r="I28" s="36" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J28" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="K28" s="100">
+      <c r="K28" s="93">
         <v>3</v>
       </c>
-      <c r="L28" s="79"/>
+      <c r="L28" s="78"/>
       <c r="M28" s="26"/>
     </row>
     <row r="29" spans="3:13" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="112">
+      <c r="C29" s="105">
         <v>26</v>
       </c>
       <c r="D29" s="38" t="s">
@@ -2677,19 +2688,19 @@
         <v>25</v>
       </c>
       <c r="I29" s="41" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J29" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="K29" s="95">
+      <c r="K29" s="88">
         <v>3</v>
       </c>
-      <c r="L29" s="79"/>
+      <c r="L29" s="78"/>
       <c r="M29" s="26"/>
     </row>
     <row r="30" spans="3:13" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="112">
+      <c r="C30" s="105">
         <v>27</v>
       </c>
       <c r="D30" s="58" t="s">
@@ -2713,14 +2724,14 @@
       <c r="J30" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="K30" s="99">
+      <c r="K30" s="92">
         <v>3</v>
       </c>
-      <c r="L30" s="79"/>
+      <c r="L30" s="78"/>
       <c r="M30" s="77"/>
     </row>
     <row r="31" spans="3:13" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C31" s="112">
+      <c r="C31" s="105">
         <v>28</v>
       </c>
       <c r="D31" s="58" t="s">
@@ -2739,52 +2750,52 @@
         <v>63</v>
       </c>
       <c r="I31" s="61" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J31" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="K31" s="99">
+      <c r="K31" s="92">
         <v>3</v>
       </c>
-      <c r="L31" s="79"/>
+      <c r="L31" s="78"/>
       <c r="M31" s="77"/>
     </row>
     <row r="32" spans="3:13" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="112">
+      <c r="C32" s="105">
         <v>29</v>
       </c>
-      <c r="D32" s="104" t="s">
+      <c r="D32" s="97" t="s">
         <v>36</v>
       </c>
-      <c r="E32" s="105" t="s">
+      <c r="E32" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="F32" s="106">
+      <c r="F32" s="99">
         <v>36393</v>
       </c>
-      <c r="G32" s="107" t="s">
+      <c r="G32" s="100" t="s">
         <v>15</v>
       </c>
-      <c r="H32" s="108" t="s">
+      <c r="H32" s="101" t="s">
         <v>38</v>
       </c>
-      <c r="I32" s="107" t="s">
-        <v>113</v>
-      </c>
-      <c r="J32" s="107" t="s">
+      <c r="I32" s="100" t="s">
+        <v>111</v>
+      </c>
+      <c r="J32" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="K32" s="109" t="s">
-        <v>135</v>
-      </c>
-      <c r="L32" s="79" t="s">
-        <v>138</v>
+      <c r="K32" s="102" t="s">
+        <v>133</v>
+      </c>
+      <c r="L32" s="78" t="s">
+        <v>136</v>
       </c>
       <c r="M32" s="77"/>
     </row>
     <row r="33" spans="3:14" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C33" s="112">
+      <c r="C33" s="105">
         <v>30</v>
       </c>
       <c r="D33" s="48" t="s">
@@ -2808,20 +2819,20 @@
       <c r="J33" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="K33" s="97" t="s">
+      <c r="K33" s="90" t="s">
+        <v>133</v>
+      </c>
+      <c r="L33" s="78" t="s">
         <v>135</v>
       </c>
-      <c r="L33" s="79" t="s">
-        <v>137</v>
-      </c>
       <c r="M33" s="77"/>
     </row>
     <row r="34" spans="3:14" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C34" s="112">
+      <c r="C34" s="105">
         <v>31</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E34" s="39" t="s">
         <v>19</v>
@@ -2841,16 +2852,16 @@
       <c r="J34" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="K34" s="95" t="s">
-        <v>135</v>
-      </c>
-      <c r="L34" s="79" t="s">
-        <v>136</v>
+      <c r="K34" s="88" t="s">
+        <v>133</v>
+      </c>
+      <c r="L34" s="78" t="s">
+        <v>134</v>
       </c>
       <c r="M34" s="77"/>
     </row>
     <row r="35" spans="3:14" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C35" s="112">
+      <c r="C35" s="105">
         <v>32</v>
       </c>
       <c r="D35" s="48" t="s">
@@ -2869,21 +2880,21 @@
         <v>69</v>
       </c>
       <c r="I35" s="41" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J35" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="K35" s="97" t="s">
-        <v>139</v>
-      </c>
-      <c r="L35" s="79" t="s">
-        <v>140</v>
+      <c r="K35" s="90" t="s">
+        <v>137</v>
+      </c>
+      <c r="L35" s="78" t="s">
+        <v>138</v>
       </c>
       <c r="M35" s="77"/>
     </row>
     <row r="36" spans="3:14" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="112">
+      <c r="C36" s="105">
         <v>33</v>
       </c>
       <c r="D36" s="43" t="s">
@@ -2907,11 +2918,11 @@
       <c r="J36" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="K36" s="96" t="s">
-        <v>139</v>
-      </c>
-      <c r="L36" s="80" t="s">
-        <v>142</v>
+      <c r="K36" s="89" t="s">
+        <v>137</v>
+      </c>
+      <c r="L36" s="79" t="s">
+        <v>140</v>
       </c>
       <c r="M36" s="77"/>
     </row>

</xml_diff>